<commit_message>
updated models with MOCI and eSeal
</commit_message>
<xml_diff>
--- a/Data/MEI.xlsx
+++ b/Data/MEI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bbecker\Projects\IandM\harborSeals\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308A75FC-AAB8-4E0F-88A9-1970B2431B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41C5C9A-4C59-49FC-80E3-9EB04E6FAB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="3195" windowWidth="22755" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEI" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
   <si>
     <t>Year</t>
   </si>
@@ -123,15 +123,24 @@
   <si>
     <t>Coyote_3yr_TP</t>
   </si>
+  <si>
+    <t>BEUTI__LAG_FEB_APR_37N_39N</t>
+  </si>
+  <si>
+    <t>MOCI_LAG_JFM_NC</t>
+  </si>
+  <si>
+    <t>eSeal_IMM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -140,6 +149,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -155,6 +165,18 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -178,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -196,8 +218,12 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +541,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X51"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -529,7 +555,7 @@
     <col min="7" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,8 +628,17 @@
       <c r="X1" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1975</v>
       </c>
@@ -652,7 +687,7 @@
       <c r="P2" s="5">
         <v>0</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="R2" s="11">
@@ -676,8 +711,17 @@
       <c r="X2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1">
       <c r="A3" s="7">
         <v>1976</v>
       </c>
@@ -750,8 +794,17 @@
       <c r="X3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="7">
         <v>1977</v>
       </c>
@@ -829,8 +882,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1">
       <c r="A5" s="7">
         <v>1978</v>
       </c>
@@ -908,8 +970,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" s="2">
         <v>1979</v>
       </c>
@@ -987,8 +1058,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="A7" s="2">
         <v>1980</v>
       </c>
@@ -1066,8 +1146,17 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" customHeight="1">
       <c r="A8" s="2">
         <v>1981</v>
       </c>
@@ -1145,8 +1234,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA8" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>1982</v>
       </c>
@@ -1224,8 +1322,17 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>1983</v>
       </c>
@@ -1303,8 +1410,17 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="A11" s="2">
         <v>1984</v>
       </c>
@@ -1382,8 +1498,17 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA11" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" customHeight="1">
       <c r="A12" s="2">
         <v>1985</v>
       </c>
@@ -1461,8 +1586,17 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA12" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>1986</v>
       </c>
@@ -1540,8 +1674,17 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA13" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>1987</v>
       </c>
@@ -1619,8 +1762,17 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA14" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="A15" s="2">
         <v>1988</v>
       </c>
@@ -1698,8 +1850,17 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA15" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="A16" s="2">
         <v>1989</v>
       </c>
@@ -1777,8 +1938,17 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y16" s="9">
+        <v>9.5595555555555549</v>
+      </c>
+      <c r="Z16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA16" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>1990</v>
       </c>
@@ -1856,8 +2026,17 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y17" s="9">
+        <v>5.8417777777777777</v>
+      </c>
+      <c r="Z17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA17" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="15.75" customHeight="1">
       <c r="A18" s="2">
         <v>1991</v>
       </c>
@@ -1935,8 +2114,17 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y18" s="9">
+        <v>12.332000000000001</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="15.75" customHeight="1">
       <c r="A19" s="2">
         <v>1992</v>
       </c>
@@ -2014,8 +2202,17 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y19" s="9">
+        <v>10.543111111111111</v>
+      </c>
+      <c r="Z19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA19" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="15.75" customHeight="1">
       <c r="A20" s="2">
         <v>1993</v>
       </c>
@@ -2093,8 +2290,17 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y20" s="9">
+        <v>0.4509999999999999</v>
+      </c>
+      <c r="Z20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA20" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>1994</v>
       </c>
@@ -2172,8 +2378,17 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y21" s="9">
+        <v>3.811666666666667</v>
+      </c>
+      <c r="Z21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA21" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="15.75" customHeight="1">
       <c r="A22" s="2">
         <v>1995</v>
       </c>
@@ -2251,8 +2466,17 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y22" s="9">
+        <v>6.4946666666666673</v>
+      </c>
+      <c r="Z22" s="9">
+        <v>0.97047871735947344</v>
+      </c>
+      <c r="AA22" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>1996</v>
       </c>
@@ -2330,8 +2554,17 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y23" s="9">
+        <v>4.8357777777777775</v>
+      </c>
+      <c r="Z23" s="9">
+        <v>7.0795726469143201</v>
+      </c>
+      <c r="AA23" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="15.75" customHeight="1">
       <c r="A24" s="2">
         <v>1997</v>
       </c>
@@ -2409,8 +2642,17 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y24" s="9">
+        <v>3.1939999999999995</v>
+      </c>
+      <c r="Z24" s="9">
+        <v>2.9412869620022999</v>
+      </c>
+      <c r="AA24" s="13">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>1998</v>
       </c>
@@ -2488,8 +2730,17 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y25" s="9">
+        <v>12.96</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>-1.8940720967417302</v>
+      </c>
+      <c r="AA25" s="13">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="15.75" customHeight="1">
       <c r="A26" s="2">
         <v>1999</v>
       </c>
@@ -2567,8 +2818,17 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y26" s="9">
+        <v>4.653777777777778</v>
+      </c>
+      <c r="Z26" s="9">
+        <v>9.923070072342739</v>
+      </c>
+      <c r="AA26" s="13">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>2000</v>
       </c>
@@ -2646,8 +2906,17 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y27" s="9">
+        <v>14.957555555555556</v>
+      </c>
+      <c r="Z27" s="9">
+        <v>-3.6211295578873948</v>
+      </c>
+      <c r="AA27" s="13">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="15.75" customHeight="1">
       <c r="A28" s="2">
         <v>2001</v>
       </c>
@@ -2725,8 +2994,17 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y28" s="9">
+        <v>8.0634444444444444</v>
+      </c>
+      <c r="Z28" s="9">
+        <v>-0.72381592762941094</v>
+      </c>
+      <c r="AA28" s="13">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>2002</v>
       </c>
@@ -2804,8 +3082,17 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y29" s="9">
+        <v>12.206333333333333</v>
+      </c>
+      <c r="Z29" s="9">
+        <v>-1.3472563024901649</v>
+      </c>
+      <c r="AA29" s="13">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" ht="15.75" customHeight="1">
       <c r="A30" s="2">
         <v>2003</v>
       </c>
@@ -2883,8 +3170,17 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y30" s="9">
+        <v>10.134333333333332</v>
+      </c>
+      <c r="Z30" s="9">
+        <v>-3.8838150861140699</v>
+      </c>
+      <c r="AA30" s="13">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>2004</v>
       </c>
@@ -2962,8 +3258,17 @@
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y31" s="9">
+        <v>5.8490000000000002</v>
+      </c>
+      <c r="Z31" s="9">
+        <v>1.9986717042991251</v>
+      </c>
+      <c r="AA31" s="13">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="2">
         <v>2005</v>
       </c>
@@ -3041,8 +3346,17 @@
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y32" s="9">
+        <v>8.113999999999999</v>
+      </c>
+      <c r="Z32" s="9">
+        <v>-1.4503325412389967E-3</v>
+      </c>
+      <c r="AA32" s="13">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>2006</v>
       </c>
@@ -3120,8 +3434,17 @@
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y33" s="9">
+        <v>4.4762222222222228</v>
+      </c>
+      <c r="Z33" s="9">
+        <v>5.2370137749712544</v>
+      </c>
+      <c r="AA33" s="13">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="2">
         <v>2007</v>
       </c>
@@ -3199,8 +3522,17 @@
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y34" s="9">
+        <v>6.7614444444444439</v>
+      </c>
+      <c r="Z34" s="9">
+        <v>0.61837497843142897</v>
+      </c>
+      <c r="AA34" s="13">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>2008</v>
       </c>
@@ -3278,8 +3610,17 @@
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y35" s="9">
+        <v>15.207222222222223</v>
+      </c>
+      <c r="Z35" s="9">
+        <v>-5.2577143948234095</v>
+      </c>
+      <c r="AA35" s="13">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" ht="15.75" customHeight="1">
       <c r="A36" s="2">
         <v>2009</v>
       </c>
@@ -3357,8 +3698,17 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y36" s="9">
+        <v>18.38977777777778</v>
+      </c>
+      <c r="Z36" s="9">
+        <v>-5.446762867435905</v>
+      </c>
+      <c r="AA36" s="13">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>2010</v>
       </c>
@@ -3436,8 +3786,17 @@
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" ht="12.75">
+      <c r="Y37" s="9">
+        <v>14.885555555555557</v>
+      </c>
+      <c r="Z37" s="9">
+        <v>-2.6176520306970152</v>
+      </c>
+      <c r="AA37" s="13">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" ht="12.75">
       <c r="A38" s="2">
         <v>2011</v>
       </c>
@@ -3515,8 +3874,17 @@
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" ht="12.75">
+      <c r="Y38" s="9">
+        <v>7.7345555555555556</v>
+      </c>
+      <c r="Z38" s="9">
+        <v>5.2378056795165904</v>
+      </c>
+      <c r="AA38" s="13">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" ht="12.75">
       <c r="A39" s="2">
         <v>2012</v>
       </c>
@@ -3594,8 +3962,17 @@
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" ht="12.75">
+      <c r="Y39" s="9">
+        <v>7.2995555555555569</v>
+      </c>
+      <c r="Z39" s="9">
+        <v>-2.3300035671537147</v>
+      </c>
+      <c r="AA39" s="13">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" ht="12.75">
       <c r="A40" s="2">
         <v>2013</v>
       </c>
@@ -3673,8 +4050,17 @@
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" ht="12.75">
+      <c r="Y40" s="9">
+        <v>9.099000000000002</v>
+      </c>
+      <c r="Z40" s="9">
+        <v>-4.2134016550613804</v>
+      </c>
+      <c r="AA40" s="13">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" ht="12.75">
       <c r="A41" s="2">
         <v>2014</v>
       </c>
@@ -3752,8 +4138,17 @@
         <f t="shared" si="38"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" ht="12.75">
+      <c r="Y41" s="9">
+        <v>20.741666666666664</v>
+      </c>
+      <c r="Z41" s="9">
+        <v>-7.2553326723331502</v>
+      </c>
+      <c r="AA41" s="13">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" ht="12.75">
       <c r="A42" s="2">
         <v>2015</v>
       </c>
@@ -3831,8 +4226,17 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y42" s="9">
+        <v>4.3252222222222221</v>
+      </c>
+      <c r="Z42" s="9">
+        <v>0.15834384455710304</v>
+      </c>
+      <c r="AA42" s="13">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>2016</v>
       </c>
@@ -3910,8 +4314,17 @@
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y43" s="9">
+        <v>7.9291111111111112</v>
+      </c>
+      <c r="Z43" s="9">
+        <v>4.1335049132677444</v>
+      </c>
+      <c r="AA43" s="13">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" ht="15.75" customHeight="1">
       <c r="A44" s="2">
         <v>2017</v>
       </c>
@@ -3989,8 +4402,17 @@
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y44" s="9">
+        <v>5.1916666666666664</v>
+      </c>
+      <c r="Z44" s="9">
+        <v>5.0773217795370051</v>
+      </c>
+      <c r="AA44" s="13">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>2018</v>
       </c>
@@ -4068,8 +4490,17 @@
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y45" s="9">
+        <v>3.7585555555555552</v>
+      </c>
+      <c r="Z45" s="9">
+        <v>3.2231984997034449</v>
+      </c>
+      <c r="AA45" s="13">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" ht="15.75" customHeight="1">
       <c r="A46" s="2">
         <v>2019</v>
       </c>
@@ -4147,8 +4578,17 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y46" s="9">
+        <v>7.9092222222222235</v>
+      </c>
+      <c r="Z46" s="9">
+        <v>-0.54326534875347898</v>
+      </c>
+      <c r="AA46" s="13">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>2020</v>
       </c>
@@ -4226,8 +4666,17 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y47" s="9">
+        <v>6.4695555555555559</v>
+      </c>
+      <c r="Z47" s="9">
+        <v>4.5047330615887997</v>
+      </c>
+      <c r="AA47" s="13">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" ht="15.75" customHeight="1">
       <c r="A48" s="2">
         <v>2021</v>
       </c>
@@ -4305,8 +4754,17 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y48" s="9">
+        <v>11.2744444444444</v>
+      </c>
+      <c r="Z48" s="9">
+        <v>-2.4508992581740099</v>
+      </c>
+      <c r="AA48" s="13">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>2022</v>
       </c>
@@ -4384,15 +4842,27 @@
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y49" s="9">
+        <v>17.934000000000001</v>
+      </c>
+      <c r="Z49" s="9">
+        <v>-4.4245947061311597</v>
+      </c>
+      <c r="AA49" s="13">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" ht="15.75" customHeight="1">
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
       <c r="Q50" s="9"/>
       <c r="R50" s="12"/>
       <c r="S50" s="11"/>
-    </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1">
+      <c r="Y50" s="9"/>
+      <c r="Z50" s="9"/>
+      <c r="AA50" s="14"/>
+    </row>
+    <row r="51" spans="1:27" ht="15.75" customHeight="1">
       <c r="R51" s="11"/>
       <c r="S51" s="11"/>
     </row>

</xml_diff>

<commit_message>
added 2023, added MOCI lags
</commit_message>
<xml_diff>
--- a/Data/MEI.xlsx
+++ b/Data/MEI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bbecker\Projects\IandM\harborSeals\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41C5C9A-4C59-49FC-80E3-9EB04E6FAB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292F7F6A-D489-475D-AD3A-AB30C6F4952A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16245" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEI" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -127,10 +127,13 @@
     <t>BEUTI__LAG_FEB_APR_37N_39N</t>
   </si>
   <si>
-    <t>MOCI_LAG_JFM_NC</t>
+    <t>eSeal_IMM</t>
   </si>
   <si>
-    <t>eSeal_IMM</t>
+    <t>MOCI_LAG_AMJ_NC</t>
+  </si>
+  <si>
+    <t>MOCI_LAG_OND_NC</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA51"/>
+  <dimension ref="A1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AC19" sqref="AC19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -555,7 +559,7 @@
     <col min="7" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,13 +636,16 @@
         <v>28</v>
       </c>
       <c r="Z1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1975</v>
       </c>
@@ -720,8 +727,11 @@
       <c r="AA2" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="7">
         <v>1976</v>
       </c>
@@ -803,8 +813,11 @@
       <c r="AA3" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB3" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="7">
         <v>1977</v>
       </c>
@@ -891,8 +904,11 @@
       <c r="AA4" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1">
       <c r="A5" s="7">
         <v>1978</v>
       </c>
@@ -979,8 +995,11 @@
       <c r="AA5" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1">
       <c r="A6" s="2">
         <v>1979</v>
       </c>
@@ -1067,8 +1086,11 @@
       <c r="AA6" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" customHeight="1">
       <c r="A7" s="2">
         <v>1980</v>
       </c>
@@ -1155,8 +1177,11 @@
       <c r="AA7" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB7" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" customHeight="1">
       <c r="A8" s="2">
         <v>1981</v>
       </c>
@@ -1243,8 +1268,11 @@
       <c r="AA8" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB8" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>1982</v>
       </c>
@@ -1331,8 +1359,11 @@
       <c r="AA9" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>1983</v>
       </c>
@@ -1419,8 +1450,11 @@
       <c r="AA10" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB10" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="15.75" customHeight="1">
       <c r="A11" s="2">
         <v>1984</v>
       </c>
@@ -1507,8 +1541,11 @@
       <c r="AA11" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB11" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1">
       <c r="A12" s="2">
         <v>1985</v>
       </c>
@@ -1595,8 +1632,11 @@
       <c r="AA12" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB12" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>1986</v>
       </c>
@@ -1683,8 +1723,11 @@
       <c r="AA13" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB13" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>1987</v>
       </c>
@@ -1771,8 +1814,11 @@
       <c r="AA14" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB14" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" customHeight="1">
       <c r="A15" s="2">
         <v>1988</v>
       </c>
@@ -1859,8 +1905,11 @@
       <c r="AA15" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB15" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="15.75" customHeight="1">
       <c r="A16" s="2">
         <v>1989</v>
       </c>
@@ -1947,8 +1996,11 @@
       <c r="AA16" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB16" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>1990</v>
       </c>
@@ -2035,8 +2087,11 @@
       <c r="AA17" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB17" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="15.75" customHeight="1">
       <c r="A18" s="2">
         <v>1991</v>
       </c>
@@ -2123,8 +2178,11 @@
       <c r="AA18" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="15.75" customHeight="1">
       <c r="A19" s="2">
         <v>1992</v>
       </c>
@@ -2211,8 +2269,11 @@
       <c r="AA19" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB19" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="15.75" customHeight="1">
       <c r="A20" s="2">
         <v>1993</v>
       </c>
@@ -2299,8 +2360,11 @@
       <c r="AA20" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB20" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>1994</v>
       </c>
@@ -2313,8 +2377,8 @@
       <c r="D21" s="5">
         <v>-1.8557885999999999</v>
       </c>
-      <c r="E21" s="9">
-        <v>0.97047871735947344</v>
+      <c r="E21" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="F21" s="9">
         <v>0.48499999999999999</v>
@@ -2387,8 +2451,11 @@
       <c r="AA21" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB21" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="15.75" customHeight="1">
       <c r="A22" s="2">
         <v>1995</v>
       </c>
@@ -2402,7 +2469,7 @@
         <v>-2.0546500999999999</v>
       </c>
       <c r="E22" s="9">
-        <v>7.0795726469143201</v>
+        <v>6.7446664188624847</v>
       </c>
       <c r="F22" s="9">
         <v>0.57099999999999995</v>
@@ -2470,13 +2537,16 @@
         <v>6.4946666666666673</v>
       </c>
       <c r="Z22" s="9">
-        <v>0.97047871735947344</v>
+        <v>-0.92108666905364545</v>
       </c>
       <c r="AA22" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB22" s="9">
+        <v>-2.6224919280831651</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>1996</v>
       </c>
@@ -2490,7 +2560,7 @@
         <v>-1.1487636999999999</v>
       </c>
       <c r="E23" s="9">
-        <v>2.9412869620022999</v>
+        <v>2.6621824353896351</v>
       </c>
       <c r="F23" s="9">
         <v>0.93200000000000005</v>
@@ -2558,13 +2628,16 @@
         <v>4.8357777777777775</v>
       </c>
       <c r="Z23" s="9">
-        <v>7.0795726469143201</v>
+        <v>1.11823863254717</v>
       </c>
       <c r="AA23" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB23" s="9">
+        <v>6.1302708184631016E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="15.75" customHeight="1">
       <c r="A24" s="2">
         <v>1997</v>
       </c>
@@ -2578,7 +2651,7 @@
         <v>-0.61802827999999999</v>
       </c>
       <c r="E24" s="9">
-        <v>-1.8940720967417302</v>
+        <v>-2.040601167241245</v>
       </c>
       <c r="F24" s="9">
         <v>0.60399999999999998</v>
@@ -2646,13 +2719,16 @@
         <v>3.1939999999999995</v>
       </c>
       <c r="Z24" s="9">
-        <v>2.9412869620022999</v>
+        <v>-0.12690858326414589</v>
       </c>
       <c r="AA24" s="13">
         <v>214</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB24" s="9">
+        <v>-6.8570742832713028E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>1998</v>
       </c>
@@ -2666,7 +2742,7 @@
         <v>0.89331784000000003</v>
       </c>
       <c r="E25" s="9">
-        <v>9.923070072342739</v>
+        <v>9.54982263107261</v>
       </c>
       <c r="F25" s="9">
         <v>1.41</v>
@@ -2734,13 +2810,16 @@
         <v>12.96</v>
       </c>
       <c r="Z25" s="9">
-        <v>-1.8940720967417302</v>
+        <v>3.6733594142763799</v>
       </c>
       <c r="AA25" s="13">
         <v>93</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB25" s="9">
+        <v>8.5579976488731599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="15.75" customHeight="1">
       <c r="A26" s="2">
         <v>1999</v>
       </c>
@@ -2754,7 +2833,7 @@
         <v>1.9742975</v>
       </c>
       <c r="E26" s="9">
-        <v>-3.6211295578873948</v>
+        <v>-3.6571146217578647</v>
       </c>
       <c r="F26" s="9">
         <v>-0.90700000000000003</v>
@@ -2822,13 +2901,16 @@
         <v>4.653777777777778</v>
       </c>
       <c r="Z26" s="9">
-        <v>9.923070072342739</v>
+        <v>5.6304880191683555</v>
       </c>
       <c r="AA26" s="13">
         <v>480</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB26" s="9">
+        <v>-4.6577690512715755</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>2000</v>
       </c>
@@ -2842,7 +2924,7 @@
         <v>2.1492676999999998</v>
       </c>
       <c r="E27" s="9">
-        <v>-0.72381592762941094</v>
+        <v>-0.80851469224483297</v>
       </c>
       <c r="F27" s="9">
         <v>-0.60499999999999998</v>
@@ -2910,13 +2992,16 @@
         <v>14.957555555555556</v>
       </c>
       <c r="Z27" s="9">
-        <v>-3.6211295578873948</v>
+        <v>-8.0540115519296958</v>
       </c>
       <c r="AA27" s="13">
         <v>343</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB27" s="9">
+        <v>-4.8450701611335507</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="15.75" customHeight="1">
       <c r="A28" s="2">
         <v>2001</v>
       </c>
@@ -2930,7 +3015,7 @@
         <v>2.3887749999999999</v>
       </c>
       <c r="E28" s="9">
-        <v>-1.3472563024901649</v>
+        <v>-1.419026724866375</v>
       </c>
       <c r="F28" s="9">
         <v>-0.192</v>
@@ -2998,13 +3083,16 @@
         <v>8.0634444444444444</v>
       </c>
       <c r="Z28" s="9">
-        <v>-0.72381592762941094</v>
+        <v>1.256784303282982</v>
       </c>
       <c r="AA28" s="13">
         <v>409</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB28" s="9">
+        <v>-3.57717553107332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>2002</v>
       </c>
@@ -3018,7 +3106,7 @@
         <v>1.8982763</v>
       </c>
       <c r="E29" s="9">
-        <v>-3.8838150861140699</v>
+        <v>-3.89141005240349</v>
       </c>
       <c r="F29" s="9">
         <v>-0.75700000000000001</v>
@@ -3086,13 +3174,16 @@
         <v>12.206333333333333</v>
       </c>
       <c r="Z29" s="9">
-        <v>-1.3472563024901649</v>
+        <v>-3.73780931891074</v>
       </c>
       <c r="AA29" s="13">
         <v>408</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB29" s="9">
+        <v>-1.1475412225254205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" ht="15.75" customHeight="1">
       <c r="A30" s="2">
         <v>2003</v>
       </c>
@@ -3106,7 +3197,7 @@
         <v>1.4907113999999999</v>
       </c>
       <c r="E30" s="9">
-        <v>1.9986717042991251</v>
+        <v>1.808592266204045</v>
       </c>
       <c r="F30" s="9">
         <v>1.0589999999999999</v>
@@ -3174,13 +3265,16 @@
         <v>10.134333333333332</v>
       </c>
       <c r="Z30" s="9">
-        <v>-3.8838150861140699</v>
+        <v>-4.4623714561606054</v>
       </c>
       <c r="AA30" s="13">
         <v>418</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB30" s="9">
+        <v>2.9821240395715352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>2004</v>
       </c>
@@ -3194,7 +3288,7 @@
         <v>0.38293237000000002</v>
       </c>
       <c r="E31" s="9">
-        <v>-1.4503325412389967E-3</v>
+        <v>-0.15069038784875349</v>
       </c>
       <c r="F31" s="9">
         <v>0.127</v>
@@ -3262,13 +3356,16 @@
         <v>5.8490000000000002</v>
       </c>
       <c r="Z31" s="9">
-        <v>1.9986717042991251</v>
+        <v>1.8229087636707599</v>
       </c>
       <c r="AA31" s="13">
         <v>492</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB31" s="9">
+        <v>0.97883518386852897</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" ht="15.75" customHeight="1">
       <c r="A32" s="2">
         <v>2005</v>
       </c>
@@ -3282,7 +3379,7 @@
         <v>-1.4269776999999999</v>
       </c>
       <c r="E32" s="9">
-        <v>5.2370137749712544</v>
+        <v>4.9125300720082299</v>
       </c>
       <c r="F32" s="9">
         <v>0.72799999999999998</v>
@@ -3350,13 +3447,16 @@
         <v>8.113999999999999</v>
       </c>
       <c r="Z32" s="9">
-        <v>-1.4503325412389967E-3</v>
+        <v>0.314466430287693</v>
       </c>
       <c r="AA32" s="13">
         <v>608</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB32" s="9">
+        <v>0.70593726610420804</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>2006</v>
       </c>
@@ -3370,7 +3470,7 @@
         <v>-0.73545015000000002</v>
       </c>
       <c r="E33" s="9">
-        <v>0.61837497843142897</v>
+        <v>0.41552462537724855</v>
       </c>
       <c r="F33" s="9">
         <v>-0.308</v>
@@ -3438,13 +3538,16 @@
         <v>4.4762222222222228</v>
       </c>
       <c r="Z33" s="9">
-        <v>5.2370137749712544</v>
+        <v>4.5971793245503498</v>
       </c>
       <c r="AA33" s="13">
         <v>674</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB33" s="9">
+        <v>-0.90814805445389657</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="15.75" customHeight="1">
       <c r="A34" s="2">
         <v>2007</v>
       </c>
@@ -3458,7 +3561,7 @@
         <v>-0.63695332999999998</v>
       </c>
       <c r="E34" s="9">
-        <v>-5.2577143948234095</v>
+        <v>-5.33793245372736</v>
       </c>
       <c r="F34" s="9">
         <v>-0.749</v>
@@ -3526,13 +3629,16 @@
         <v>6.7614444444444439</v>
       </c>
       <c r="Z34" s="9">
-        <v>0.61837497843142897</v>
+        <v>4.9054919553647247</v>
       </c>
       <c r="AA34" s="13">
         <v>831</v>
       </c>
-    </row>
-    <row r="35" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB34" s="9">
+        <v>-0.70288069056732705</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>2008</v>
       </c>
@@ -3546,7 +3652,7 @@
         <v>1.3266521</v>
       </c>
       <c r="E35" s="9">
-        <v>-5.446762867435905</v>
+        <v>-5.455950860383215</v>
       </c>
       <c r="F35" s="9">
         <v>-1.125</v>
@@ -3614,13 +3720,16 @@
         <v>15.207222222222223</v>
       </c>
       <c r="Z35" s="9">
-        <v>-5.2577143948234095</v>
+        <v>-4.3319024391373304</v>
       </c>
       <c r="AA35" s="13">
         <v>516</v>
       </c>
-    </row>
-    <row r="36" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB35" s="9">
+        <v>-5.3832213694813404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" ht="15.75" customHeight="1">
       <c r="A36" s="2">
         <v>2009</v>
       </c>
@@ -3634,7 +3743,7 @@
         <v>6.0374695999999999E-2</v>
       </c>
       <c r="E36" s="9">
-        <v>-2.6176520306970152</v>
+        <v>-2.6963315103198049</v>
       </c>
       <c r="F36" s="9">
         <v>-1.8620000000000001</v>
@@ -3702,13 +3811,16 @@
         <v>18.38977777777778</v>
       </c>
       <c r="Z36" s="9">
-        <v>-5.446762867435905</v>
+        <v>-6.6667644212892396</v>
       </c>
       <c r="AA36" s="13">
         <v>653</v>
       </c>
-    </row>
-    <row r="37" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB36" s="9">
+        <v>-2.9854484174399847</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>2010</v>
       </c>
@@ -3722,7 +3834,7 @@
         <v>1.6520432</v>
       </c>
       <c r="E37" s="9">
-        <v>5.2378056795165904</v>
+        <v>4.9953522875093253</v>
       </c>
       <c r="F37" s="9">
         <v>-4.4999999999999998E-2</v>
@@ -3790,13 +3902,16 @@
         <v>14.885555555555557</v>
       </c>
       <c r="Z37" s="9">
-        <v>-2.6176520306970152</v>
+        <v>-0.75959971101834345</v>
       </c>
       <c r="AA37" s="13">
         <v>433</v>
       </c>
-    </row>
-    <row r="38" spans="1:27" ht="12.75">
+      <c r="AB37" s="9">
+        <v>-3.9593844720987009E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="12.75">
       <c r="A38" s="2">
         <v>2011</v>
       </c>
@@ -3810,7 +3925,7 @@
         <v>1.1446472999999999</v>
       </c>
       <c r="E38" s="9">
-        <v>-2.3300035671537147</v>
+        <v>-2.3983499754499151</v>
       </c>
       <c r="F38" s="9">
         <v>-1.0740000000000001</v>
@@ -3878,13 +3993,16 @@
         <v>7.7345555555555556</v>
       </c>
       <c r="Z38" s="9">
-        <v>5.2378056795165904</v>
+        <v>-1.5664581156725255</v>
       </c>
       <c r="AA38" s="13">
         <v>719</v>
       </c>
-    </row>
-    <row r="39" spans="1:27" ht="12.75">
+      <c r="AB38" s="9">
+        <v>-1.4158059488818469</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="12.75">
       <c r="A39" s="2">
         <v>2012</v>
       </c>
@@ -3898,7 +4016,7 @@
         <v>1.0337715999999999</v>
       </c>
       <c r="E39" s="9">
-        <v>-4.2134016550613804</v>
+        <v>-4.2534663878926349</v>
       </c>
       <c r="F39" s="9">
         <v>-1.4319999999999999</v>
@@ -3966,13 +4084,16 @@
         <v>7.2995555555555569</v>
       </c>
       <c r="Z39" s="9">
-        <v>-2.3300035671537147</v>
+        <v>-1.8991672842734699</v>
       </c>
       <c r="AA39" s="13">
         <v>753</v>
       </c>
-    </row>
-    <row r="40" spans="1:27" ht="12.75">
+      <c r="AB39" s="9">
+        <v>-3.94158080668281</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" ht="12.75">
       <c r="A40" s="2">
         <v>2013</v>
       </c>
@@ -3986,7 +4107,7 @@
         <v>0.69234249000000003</v>
       </c>
       <c r="E40" s="9">
-        <v>-7.2553326723331502</v>
+        <v>-7.244695029631635</v>
       </c>
       <c r="F40" s="9">
         <v>-1.115</v>
@@ -4054,13 +4175,16 @@
         <v>9.099000000000002</v>
       </c>
       <c r="Z40" s="9">
-        <v>-4.2134016550613804</v>
+        <v>-2.448511848603375</v>
       </c>
       <c r="AA40" s="13">
         <v>826</v>
       </c>
-    </row>
-    <row r="41" spans="1:27" ht="12.75">
+      <c r="AB40" s="9">
+        <v>2.6823130452793751</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" ht="12.75">
       <c r="A41" s="2">
         <v>2014</v>
       </c>
@@ -4074,7 +4198,7 @@
         <v>-0.38445781000000001</v>
       </c>
       <c r="E41" s="9">
-        <v>0.15834384455710304</v>
+        <v>-1.3094809882834957E-2</v>
       </c>
       <c r="F41" s="9">
         <v>0.42599999999999999</v>
@@ -4142,13 +4266,16 @@
         <v>20.741666666666664</v>
       </c>
       <c r="Z41" s="9">
-        <v>-7.2553326723331502</v>
+        <v>-2.8938079755209851</v>
       </c>
       <c r="AA41" s="13">
         <v>880</v>
       </c>
-    </row>
-    <row r="42" spans="1:27" ht="12.75">
+      <c r="AB41" s="9">
+        <v>-4.9758346309216446</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" ht="12.75">
       <c r="A42" s="2">
         <v>2015</v>
       </c>
@@ -4162,7 +4289,7 @@
         <v>-1.2847062</v>
       </c>
       <c r="E42" s="9">
-        <v>4.1335049132677444</v>
+        <v>3.820008075183305</v>
       </c>
       <c r="F42" s="9">
         <v>1.3260000000000001</v>
@@ -4230,13 +4357,16 @@
         <v>4.3252222222222221</v>
       </c>
       <c r="Z42" s="9">
-        <v>0.15834384455710304</v>
+        <v>1.40123084918149</v>
       </c>
       <c r="AA42" s="13">
         <v>777</v>
       </c>
-    </row>
-    <row r="43" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB42" s="9">
+        <v>8.728865487872115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>2016</v>
       </c>
@@ -4250,7 +4380,7 @@
         <v>0.62255843</v>
       </c>
       <c r="E43" s="9">
-        <v>5.0773217795370051</v>
+        <v>4.7893623725614951</v>
       </c>
       <c r="F43" s="9">
         <v>1.571</v>
@@ -4318,13 +4448,16 @@
         <v>7.9291111111111112</v>
       </c>
       <c r="Z43" s="9">
-        <v>4.1335049132677444</v>
+        <v>3.9882261960460097</v>
       </c>
       <c r="AA43" s="13">
         <v>825</v>
       </c>
-    </row>
-    <row r="44" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB43" s="9">
+        <v>4.6032079036796496</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" ht="15.75" customHeight="1">
       <c r="A44" s="2">
         <v>2017</v>
       </c>
@@ -4338,7 +4471,7 @@
         <v>-0.84995303</v>
       </c>
       <c r="E44" s="9">
-        <v>3.2231984997034449</v>
+        <v>2.9302599540205998</v>
       </c>
       <c r="F44" s="9">
         <v>3.3000000000000002E-2</v>
@@ -4391,7 +4524,7 @@
         <v>3</v>
       </c>
       <c r="V44" s="5">
-        <f t="shared" si="41"/>
+        <f>SUM(I42:I44)</f>
         <v>2</v>
       </c>
       <c r="W44" s="5">
@@ -4406,13 +4539,16 @@
         <v>5.1916666666666664</v>
       </c>
       <c r="Z44" s="9">
-        <v>5.0773217795370051</v>
+        <v>3.7462448286140551</v>
       </c>
       <c r="AA44" s="13">
         <v>703</v>
       </c>
-    </row>
-    <row r="45" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB44" s="9">
+        <v>2.6078631351677197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>2018</v>
       </c>
@@ -4426,7 +4562,7 @@
         <v>-2.0866373</v>
       </c>
       <c r="E45" s="9">
-        <v>-0.54326534875347898</v>
+        <v>-0.75040579319026557</v>
       </c>
       <c r="F45" s="9">
         <v>-0.77800000000000002</v>
@@ -4494,13 +4630,16 @@
         <v>3.7585555555555552</v>
       </c>
       <c r="Z45" s="9">
-        <v>3.2231984997034449</v>
+        <v>2.4873387255813197</v>
       </c>
       <c r="AA45" s="13">
         <v>1092</v>
       </c>
-    </row>
-    <row r="46" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB45" s="9">
+        <v>-0.32915289173666251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="15.75" customHeight="1">
       <c r="A46" s="2">
         <v>2019</v>
       </c>
@@ -4514,7 +4653,7 @@
         <v>-1.9816495999999999</v>
       </c>
       <c r="E46" s="9">
-        <v>4.5047330615887997</v>
+        <v>4.2048198393530098</v>
       </c>
       <c r="F46" s="9">
         <v>-0.313</v>
@@ -4582,13 +4721,16 @@
         <v>7.9092222222222235</v>
       </c>
       <c r="Z46" s="9">
-        <v>-0.54326534875347898</v>
+        <v>0.37488515661695349</v>
       </c>
       <c r="AA46" s="13">
         <v>941</v>
       </c>
-    </row>
-    <row r="47" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB46" s="9">
+        <v>2.5213020526908831</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>2020</v>
       </c>
@@ -4602,7 +4744,7 @@
         <v>-1.9382005</v>
       </c>
       <c r="E47" s="9">
-        <v>-2.4508992581740099</v>
+        <v>-2.6092509175834051</v>
       </c>
       <c r="F47" s="9">
         <v>-1.6439999999999999</v>
@@ -4670,13 +4812,16 @@
         <v>6.4695555555555559</v>
       </c>
       <c r="Z47" s="9">
-        <v>4.5047330615887997</v>
+        <v>5.6784310454138645</v>
       </c>
       <c r="AA47" s="13">
         <v>1058</v>
       </c>
-    </row>
-    <row r="48" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB47" s="9">
+        <v>2.0080743350620982</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" ht="15.75" customHeight="1">
       <c r="A48" s="2">
         <v>2021</v>
       </c>
@@ -4690,7 +4835,7 @@
         <v>-0.84696722999999996</v>
       </c>
       <c r="E48" s="9">
-        <v>-4.4245947061311597</v>
+        <v>-4.5217274613466349</v>
       </c>
       <c r="F48" s="9">
         <v>-1.601</v>
@@ -4758,13 +4903,16 @@
         <v>11.2744444444444</v>
       </c>
       <c r="Z48" s="9">
-        <v>-2.4508992581740099</v>
+        <v>3.0639952044373198</v>
       </c>
       <c r="AA48" s="13">
         <v>1129</v>
       </c>
-    </row>
-    <row r="49" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB48" s="9">
+        <v>-3.5344920110967797</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>2022</v>
       </c>
@@ -4778,7 +4926,7 @@
         <v>-1.1043676</v>
       </c>
       <c r="E49" s="9">
-        <v>-4.8495120329289749</v>
+        <v>-4.9584526960541551</v>
       </c>
       <c r="F49" s="9">
         <v>-1.5720000000000001</v>
@@ -4831,7 +4979,7 @@
         <v>3</v>
       </c>
       <c r="V49" s="5">
-        <f t="shared" si="46"/>
+        <f>SUM(I47:I49)</f>
         <v>2</v>
       </c>
       <c r="W49" s="5">
@@ -4846,23 +4994,107 @@
         <v>17.934000000000001</v>
       </c>
       <c r="Z49" s="9">
-        <v>-4.4245947061311597</v>
+        <v>-2.7682281116995551</v>
       </c>
       <c r="AA49" s="13">
         <v>1256</v>
       </c>
-    </row>
-    <row r="50" spans="1:27" ht="15.75" customHeight="1">
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="Q50" s="9"/>
-      <c r="R50" s="12"/>
-      <c r="S50" s="11"/>
-      <c r="Y50" s="9"/>
-      <c r="Z50" s="9"/>
-      <c r="AA50" s="14"/>
-    </row>
-    <row r="51" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AB49" s="9">
+        <v>-0.11571873430508575</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A50" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="9">
+        <v>-0.4428782783124115</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="5">
+        <v>1</v>
+      </c>
+      <c r="H50" s="5">
+        <v>1</v>
+      </c>
+      <c r="I50" s="5">
+        <v>1</v>
+      </c>
+      <c r="J50" s="5">
+        <v>0</v>
+      </c>
+      <c r="K50" s="5">
+        <v>0</v>
+      </c>
+      <c r="L50" t="s">
+        <v>6</v>
+      </c>
+      <c r="M50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="T50" s="5">
+        <f>SUM(G48:G50)</f>
+        <v>1</v>
+      </c>
+      <c r="U50" s="5">
+        <f t="shared" ref="U50" si="47">SUM(H48:H50)</f>
+        <v>3</v>
+      </c>
+      <c r="V50" s="5">
+        <f>SUM(I48:I50)</f>
+        <v>3</v>
+      </c>
+      <c r="W50" s="5">
+        <f t="shared" ref="W50" si="48">SUM(J48:J50)</f>
+        <v>0</v>
+      </c>
+      <c r="X50" s="5">
+        <f t="shared" ref="X50" si="49">SUM(K48:K50)</f>
+        <v>0</v>
+      </c>
+      <c r="Y50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z50" s="9">
+        <v>-4.2022302358251196</v>
+      </c>
+      <c r="AA50" s="14">
+        <v>1200</v>
+      </c>
+      <c r="AB50" s="9">
+        <v>-1.52761457526795</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" ht="15.75" customHeight="1">
       <c r="R51" s="11"/>
       <c r="S51" s="11"/>
     </row>

</xml_diff>

<commit_message>
Update 2023 data and new coyote index
</commit_message>
<xml_diff>
--- a/Data/MEI.xlsx
+++ b/Data/MEI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bbecker\Projects\IandM\harborSeals\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292F7F6A-D489-475D-AD3A-AB30C6F4952A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E324A8-94A9-4776-8086-16CEDD87C430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16245" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="25725" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEI" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -59,21 +59,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Coyote_BL</t>
-  </si>
-  <si>
-    <t>Coyote_DP</t>
-  </si>
-  <si>
-    <t>Coyote_DE</t>
-  </si>
-  <si>
-    <t>Coyote_TB</t>
-  </si>
-  <si>
-    <t>Coyote_TP</t>
   </si>
   <si>
     <t>Coyote_DP_rate</t>
@@ -135,15 +120,31 @@
   <si>
     <t>MOCI_LAG_OND_NC</t>
   </si>
+  <si>
+    <t>Coyote_BL_3yr</t>
+  </si>
+  <si>
+    <t>Coyote_DE_3yr</t>
+  </si>
+  <si>
+    <t>Coyote_DP_3yr</t>
+  </si>
+  <si>
+    <t>Coyote_TB_3yr</t>
+  </si>
+  <si>
+    <t>Coyote_TP_3yr</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -168,18 +169,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -223,10 +212,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,9 +533,9 @@
   </sheetPr>
   <dimension ref="A1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -556,7 +543,8 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="4" width="12" customWidth="1"/>
     <col min="5" max="6" width="17" customWidth="1"/>
-    <col min="7" max="11" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1">
@@ -570,79 +558,79 @@
         <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="U1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
@@ -836,19 +824,24 @@
       <c r="F4" s="9">
         <v>0.73199999999999998</v>
       </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
+      <c r="G4" s="14">
+        <f>AVERAGE(0.2*L2,0.3*L3,0.5*L4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="14">
+        <f>AVERAGE(0.2*M2,0.3*M3,0.5*M4)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <f>AVERAGE(0.2*N2,0.3*N3,0.5*N4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" ref="J4:K50" si="0">AVERAGE(0.2*O2,0.3*O3,0.5*O4)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4" s="5">
@@ -880,19 +873,19 @@
         <v>0</v>
       </c>
       <c r="U4" s="5">
-        <f t="shared" ref="U4:X4" si="0">SUM(H2:H4)</f>
+        <f t="shared" ref="U4:X4" si="1">SUM(H2:H4)</f>
         <v>0</v>
       </c>
       <c r="V4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y4" t="s">
@@ -927,19 +920,24 @@
       <c r="F5" s="9">
         <v>1.3919999999999999</v>
       </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
+      <c r="G5" s="14">
+        <f t="shared" ref="G5:G50" si="2">AVERAGE(0.2*L3,0.3*L4,0.5*L5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" ref="H5:H50" si="3">AVERAGE(0.2*M3,0.3*M4,0.5*M5)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" ref="I5:I50" si="4">AVERAGE(0.2*N3,0.3*N4,0.5*N5)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="5">
@@ -967,23 +965,23 @@
         <v>119.33333333333333</v>
       </c>
       <c r="T5" s="5">
-        <f t="shared" ref="T5:T49" si="1">SUM(G3:G5)</f>
+        <f t="shared" ref="T5:T49" si="5">SUM(G3:G5)</f>
         <v>0</v>
       </c>
       <c r="U5" s="5">
-        <f t="shared" ref="U5:X5" si="2">SUM(H3:H5)</f>
+        <f t="shared" ref="U5:X5" si="6">SUM(H3:H5)</f>
         <v>0</v>
       </c>
       <c r="V5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Y5" t="s">
@@ -1018,19 +1016,24 @@
       <c r="F6" s="9">
         <v>-0.29799999999999999</v>
       </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
+      <c r="G6" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L6" s="5">
@@ -1058,23 +1061,23 @@
         <v>108.66666666666667</v>
       </c>
       <c r="T6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U6" s="5">
-        <f t="shared" ref="U6:X6" si="3">SUM(H4:H6)</f>
+        <f t="shared" ref="U6:X6" si="7">SUM(H4:H6)</f>
         <v>0</v>
       </c>
       <c r="V6" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W6" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X6" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y6" t="s">
@@ -1109,19 +1112,24 @@
       <c r="F7" s="9">
         <v>0.90400000000000003</v>
       </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
+      <c r="G7" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L7" s="5">
@@ -1149,23 +1157,23 @@
         <v>97.666666666666671</v>
       </c>
       <c r="T7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U7" s="5">
-        <f t="shared" ref="U7:X7" si="4">SUM(H5:H7)</f>
+        <f t="shared" ref="U7:X7" si="8">SUM(H5:H7)</f>
         <v>0</v>
       </c>
       <c r="V7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y7" t="s">
@@ -1200,19 +1208,24 @@
       <c r="F8" s="9">
         <v>1.486</v>
       </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
+      <c r="G8" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L8" s="5">
@@ -1240,23 +1253,23 @@
         <v>139</v>
       </c>
       <c r="T8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U8" s="5">
-        <f t="shared" ref="U8:X8" si="5">SUM(H6:H8)</f>
+        <f t="shared" ref="U8:X8" si="9">SUM(H6:H8)</f>
         <v>0</v>
       </c>
       <c r="V8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y8" t="s">
@@ -1291,19 +1304,24 @@
       <c r="F9" s="9">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
+      <c r="G9" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L9" s="5">
@@ -1331,23 +1349,23 @@
         <v>155</v>
       </c>
       <c r="T9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U9" s="5">
-        <f t="shared" ref="U9:X9" si="6">SUM(H7:H9)</f>
+        <f t="shared" ref="U9:X9" si="10">SUM(H7:H9)</f>
         <v>0</v>
       </c>
       <c r="V9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="W9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="X9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Y9" t="s">
@@ -1382,19 +1400,24 @@
       <c r="F10" s="9">
         <v>1.8129999999999999</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
+      <c r="G10" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L10" s="5">
@@ -1422,23 +1445,23 @@
         <v>114.33333333333333</v>
       </c>
       <c r="T10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U10" s="5">
-        <f t="shared" ref="U10:X10" si="7">SUM(H8:H10)</f>
+        <f t="shared" ref="U10:X10" si="11">SUM(H8:H10)</f>
         <v>0</v>
       </c>
       <c r="V10" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W10" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="X10" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Y10" t="s">
@@ -1473,19 +1496,24 @@
       <c r="F11" s="9">
         <v>1.4610000000000001</v>
       </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
+      <c r="G11" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L11" s="5">
@@ -1513,23 +1541,23 @@
         <v>23</v>
       </c>
       <c r="T11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U11" s="5">
-        <f t="shared" ref="U11:X11" si="8">SUM(H9:H11)</f>
+        <f t="shared" ref="U11:X11" si="12">SUM(H9:H11)</f>
         <v>0</v>
       </c>
       <c r="V11" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W11" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X11" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Y11" t="s">
@@ -1564,19 +1592,24 @@
       <c r="F12" s="9">
         <v>-6.4000000000000001E-2</v>
       </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
+      <c r="G12" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L12" s="5">
@@ -1604,23 +1637,23 @@
         <v>99.333333333333329</v>
       </c>
       <c r="T12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U12" s="5">
-        <f t="shared" ref="U12:X12" si="9">SUM(H10:H12)</f>
+        <f t="shared" ref="U12:X12" si="13">SUM(H10:H12)</f>
         <v>0</v>
       </c>
       <c r="V12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="W12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="X12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Y12" t="s">
@@ -1655,19 +1688,24 @@
       <c r="F13" s="9">
         <v>1.9930000000000001</v>
       </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0</v>
-      </c>
-      <c r="K13" s="5">
+      <c r="G13" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L13" s="5">
@@ -1695,23 +1733,23 @@
         <v>90.333333333333329</v>
       </c>
       <c r="T13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U13" s="5">
-        <f t="shared" ref="U13:X13" si="10">SUM(H11:H13)</f>
+        <f t="shared" ref="U13:X13" si="14">SUM(H11:H13)</f>
         <v>0</v>
       </c>
       <c r="V13" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="W13" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X13" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y13" t="s">
@@ -1746,19 +1784,24 @@
       <c r="F14" s="9">
         <v>1.5840000000000001</v>
       </c>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
+      <c r="G14" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L14" s="5">
@@ -1786,23 +1829,23 @@
         <v>83</v>
       </c>
       <c r="T14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U14" s="5">
-        <f t="shared" ref="U14:X14" si="11">SUM(H12:H14)</f>
+        <f t="shared" ref="U14:X14" si="15">SUM(H12:H14)</f>
         <v>0</v>
       </c>
       <c r="V14" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W14" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X14" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y14" t="s">
@@ -1837,19 +1880,24 @@
       <c r="F15" s="9">
         <v>0.63900000000000001</v>
       </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-      <c r="K15" s="5">
+      <c r="G15" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L15" s="5">
@@ -1877,23 +1925,23 @@
         <v>82.666666666666671</v>
       </c>
       <c r="T15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U15" s="5">
-        <f t="shared" ref="U15:X15" si="12">SUM(H13:H15)</f>
+        <f t="shared" ref="U15:X15" si="16">SUM(H13:H15)</f>
         <v>0</v>
       </c>
       <c r="V15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Y15" t="s">
@@ -1928,19 +1976,24 @@
       <c r="F16" s="9">
         <v>-0.95799999999999996</v>
       </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5">
+      <c r="G16" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L16" s="5">
@@ -1968,23 +2021,23 @@
         <v>72</v>
       </c>
       <c r="T16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U16" s="5">
-        <f t="shared" ref="U16:X16" si="13">SUM(H14:H16)</f>
+        <f t="shared" ref="U16:X16" si="17">SUM(H14:H16)</f>
         <v>0</v>
       </c>
       <c r="V16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="W16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Y16" s="9">
@@ -2019,19 +2072,24 @@
       <c r="F17" s="9">
         <v>-0.78200000000000003</v>
       </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
+      <c r="G17" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L17" s="5">
@@ -2059,23 +2117,23 @@
         <v>62</v>
       </c>
       <c r="T17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U17" s="5">
-        <f t="shared" ref="U17:X17" si="14">SUM(H15:H17)</f>
+        <f t="shared" ref="U17:X17" si="18">SUM(H15:H17)</f>
         <v>0</v>
       </c>
       <c r="V17" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="W17" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="X17" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Y17" s="9">
@@ -2110,19 +2168,24 @@
       <c r="F18" s="9">
         <v>-0.77200000000000002</v>
       </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
+      <c r="G18" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L18" s="5">
@@ -2150,23 +2213,23 @@
         <v>67.666666666666671</v>
       </c>
       <c r="T18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U18" s="5">
-        <f t="shared" ref="U18:X18" si="15">SUM(H16:H18)</f>
+        <f t="shared" ref="U18:X18" si="19">SUM(H16:H18)</f>
         <v>0</v>
       </c>
       <c r="V18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y18" s="9">
@@ -2201,19 +2264,24 @@
       <c r="F19" s="9">
         <v>0.27400000000000002</v>
       </c>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
+      <c r="G19" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L19" s="5">
@@ -2241,23 +2309,23 @@
         <v>123.66666666666667</v>
       </c>
       <c r="T19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U19" s="5">
-        <f t="shared" ref="U19:X19" si="16">SUM(H17:H19)</f>
+        <f t="shared" ref="U19:X19" si="20">SUM(H17:H19)</f>
         <v>0</v>
       </c>
       <c r="V19" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="W19" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X19" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Y19" s="9">
@@ -2292,19 +2360,24 @@
       <c r="F20" s="9">
         <v>0.62</v>
       </c>
-      <c r="G20" s="5">
-        <v>0</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5">
+      <c r="G20" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L20" s="5">
@@ -2332,23 +2405,23 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U20" s="5">
-        <f t="shared" ref="U20:X20" si="17">SUM(H18:H20)</f>
+        <f t="shared" ref="U20:X20" si="21">SUM(H18:H20)</f>
         <v>0</v>
       </c>
       <c r="V20" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="W20" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="X20" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Y20" s="9">
@@ -2383,19 +2456,24 @@
       <c r="F21" s="9">
         <v>0.48499999999999999</v>
       </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0</v>
-      </c>
-      <c r="K21" s="5">
+      <c r="G21" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L21" s="5">
@@ -2423,23 +2501,23 @@
         <v>12.666666666666666</v>
       </c>
       <c r="T21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U21" s="5">
-        <f t="shared" ref="U21:X21" si="18">SUM(H19:H21)</f>
+        <f t="shared" ref="U21:X21" si="22">SUM(H19:H21)</f>
         <v>0</v>
       </c>
       <c r="V21" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W21" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="X21" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="Y21" s="9">
@@ -2474,19 +2552,24 @@
       <c r="F22" s="9">
         <v>0.57099999999999995</v>
       </c>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
-        <v>0</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
+      <c r="G22" s="14">
+        <f>AVERAGE(0.2*L20,0.3*L21,0.5*L22)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L22" s="5">
@@ -2514,23 +2597,23 @@
         <v>99.333333333333329</v>
       </c>
       <c r="T22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U22" s="5">
-        <f t="shared" ref="U22:X22" si="19">SUM(H20:H22)</f>
+        <f t="shared" ref="U22:X22" si="23">SUM(H20:H22)</f>
         <v>0</v>
       </c>
       <c r="V22" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W22" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="X22" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="Y22" s="9">
@@ -2565,19 +2648,24 @@
       <c r="F23" s="9">
         <v>0.93200000000000005</v>
       </c>
-      <c r="G23" s="5">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5">
+      <c r="G23" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L23" s="5">
@@ -2605,23 +2693,23 @@
         <v>71.333333333333329</v>
       </c>
       <c r="T23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U23" s="5">
-        <f t="shared" ref="U23:X23" si="20">SUM(H21:H23)</f>
+        <f t="shared" ref="U23:X23" si="24">SUM(H21:H23)</f>
         <v>0</v>
       </c>
       <c r="V23" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="W23" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="X23" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Y23" s="9">
@@ -2656,19 +2744,24 @@
       <c r="F24" s="9">
         <v>0.60399999999999998</v>
       </c>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5">
-        <v>0</v>
-      </c>
-      <c r="J24" s="5">
-        <v>0</v>
-      </c>
-      <c r="K24" s="5">
+      <c r="G24" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L24" s="5">
@@ -2696,23 +2789,23 @@
         <v>63.333333333333336</v>
       </c>
       <c r="T24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U24" s="5">
-        <f t="shared" ref="U24:X24" si="21">SUM(H22:H24)</f>
+        <f t="shared" ref="U24:X24" si="25">SUM(H22:H24)</f>
         <v>0</v>
       </c>
       <c r="V24" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W24" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="X24" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Y24" s="9">
@@ -2721,7 +2814,7 @@
       <c r="Z24" s="9">
         <v>-0.12690858326414589</v>
       </c>
-      <c r="AA24" s="13">
+      <c r="AA24">
         <v>214</v>
       </c>
       <c r="AB24" s="9">
@@ -2747,19 +2840,24 @@
       <c r="F25" s="9">
         <v>1.41</v>
       </c>
-      <c r="G25" s="5">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5">
-        <v>0</v>
-      </c>
-      <c r="K25" s="5">
+      <c r="G25" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L25" s="5">
@@ -2787,23 +2885,23 @@
         <v>79.333333333333329</v>
       </c>
       <c r="T25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U25" s="5">
-        <f t="shared" ref="U25:X25" si="22">SUM(H23:H25)</f>
+        <f t="shared" ref="U25:X25" si="26">SUM(H23:H25)</f>
         <v>0</v>
       </c>
       <c r="V25" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="W25" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="X25" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="Y25" s="9">
@@ -2812,8 +2910,8 @@
       <c r="Z25" s="9">
         <v>3.6733594142763799</v>
       </c>
-      <c r="AA25" s="13">
-        <v>93</v>
+      <c r="AA25">
+        <v>111</v>
       </c>
       <c r="AB25" s="9">
         <v>8.5579976488731599</v>
@@ -2838,19 +2936,24 @@
       <c r="F26" s="9">
         <v>-0.90700000000000003</v>
       </c>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5">
-        <v>0</v>
-      </c>
-      <c r="J26" s="5">
-        <v>0</v>
-      </c>
-      <c r="K26" s="5">
+      <c r="G26" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L26" s="5">
@@ -2878,23 +2981,23 @@
         <v>53.333333333333336</v>
       </c>
       <c r="T26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U26" s="5">
-        <f t="shared" ref="U26:X26" si="23">SUM(H24:H26)</f>
+        <f t="shared" ref="U26:X26" si="27">SUM(H24:H26)</f>
         <v>0</v>
       </c>
       <c r="V26" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="W26" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="X26" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Y26" s="9">
@@ -2903,8 +3006,8 @@
       <c r="Z26" s="9">
         <v>5.6304880191683555</v>
       </c>
-      <c r="AA26" s="13">
-        <v>480</v>
+      <c r="AA26">
+        <v>488</v>
       </c>
       <c r="AB26" s="9">
         <v>-4.6577690512715755</v>
@@ -2929,19 +3032,24 @@
       <c r="F27" s="9">
         <v>-0.60499999999999998</v>
       </c>
-      <c r="G27" s="5">
-        <v>0</v>
-      </c>
-      <c r="H27" s="5">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
-        <v>0</v>
-      </c>
-      <c r="K27" s="5">
+      <c r="G27" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L27" s="5">
@@ -2969,23 +3077,23 @@
         <v>221.33333333333334</v>
       </c>
       <c r="T27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U27" s="5">
-        <f t="shared" ref="U27:X27" si="24">SUM(H25:H27)</f>
+        <f t="shared" ref="U27:X27" si="28">SUM(H25:H27)</f>
         <v>0</v>
       </c>
       <c r="V27" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="W27" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="X27" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Y27" s="9">
@@ -2994,8 +3102,8 @@
       <c r="Z27" s="9">
         <v>-8.0540115519296958</v>
       </c>
-      <c r="AA27" s="13">
-        <v>343</v>
+      <c r="AA27">
+        <v>365</v>
       </c>
       <c r="AB27" s="9">
         <v>-4.8450701611335507</v>
@@ -3020,19 +3128,24 @@
       <c r="F28" s="9">
         <v>-0.192</v>
       </c>
-      <c r="G28" s="5">
-        <v>0</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0</v>
-      </c>
-      <c r="I28" s="5">
-        <v>0</v>
-      </c>
-      <c r="J28" s="5">
-        <v>0</v>
-      </c>
-      <c r="K28" s="5">
+      <c r="G28" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L28" s="5">
@@ -3060,23 +3173,23 @@
         <v>80.666666666666671</v>
       </c>
       <c r="T28" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U28" s="5">
-        <f t="shared" ref="U28:X28" si="25">SUM(H26:H28)</f>
+        <f t="shared" ref="U28:X28" si="29">SUM(H26:H28)</f>
         <v>0</v>
       </c>
       <c r="V28" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="W28" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="X28" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="Y28" s="9">
@@ -3085,8 +3198,8 @@
       <c r="Z28" s="9">
         <v>1.256784303282982</v>
       </c>
-      <c r="AA28" s="13">
-        <v>409</v>
+      <c r="AA28">
+        <v>413</v>
       </c>
       <c r="AB28" s="9">
         <v>-3.57717553107332</v>
@@ -3111,19 +3224,24 @@
       <c r="F29" s="9">
         <v>-0.75700000000000001</v>
       </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5">
-        <v>0</v>
-      </c>
-      <c r="I29" s="5">
-        <v>0</v>
-      </c>
-      <c r="J29" s="5">
-        <v>0</v>
-      </c>
-      <c r="K29" s="5">
+      <c r="G29" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L29" s="5">
@@ -3151,23 +3269,23 @@
         <v>156.33333333333334</v>
       </c>
       <c r="T29" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U29" s="5">
-        <f t="shared" ref="U29:X29" si="26">SUM(H27:H29)</f>
+        <f t="shared" ref="U29:X29" si="30">SUM(H27:H29)</f>
         <v>0</v>
       </c>
       <c r="V29" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="W29" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="X29" s="5">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="Y29" s="9">
@@ -3176,8 +3294,8 @@
       <c r="Z29" s="9">
         <v>-3.73780931891074</v>
       </c>
-      <c r="AA29" s="13">
-        <v>408</v>
+      <c r="AA29">
+        <v>414</v>
       </c>
       <c r="AB29" s="9">
         <v>-1.1475412225254205</v>
@@ -3202,26 +3320,31 @@
       <c r="F30" s="9">
         <v>1.0589999999999999</v>
       </c>
-      <c r="G30" s="5">
-        <v>0</v>
-      </c>
-      <c r="H30" s="5">
-        <v>1</v>
-      </c>
-      <c r="I30" s="5">
-        <v>1</v>
-      </c>
-      <c r="J30" s="5">
-        <v>0</v>
-      </c>
-      <c r="K30" s="5">
+      <c r="G30" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="14">
+        <f t="shared" si="3"/>
+        <v>3.6231884057971015E-3</v>
+      </c>
+      <c r="I30" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L30" s="5">
         <v>0</v>
       </c>
       <c r="M30" s="5">
-        <v>0.02</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="N30" s="5">
         <v>0</v>
@@ -3242,23 +3365,23 @@
         <v>117.33333333333333</v>
       </c>
       <c r="T30" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U30" s="5">
-        <f t="shared" ref="U30:X30" si="27">SUM(H28:H30)</f>
-        <v>1</v>
+        <f t="shared" ref="U30:X30" si="31">SUM(H28:H30)</f>
+        <v>3.6231884057971015E-3</v>
       </c>
       <c r="V30" s="5">
-        <f t="shared" si="27"/>
-        <v>1</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="W30" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="X30" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="Y30" s="9">
@@ -3267,8 +3390,8 @@
       <c r="Z30" s="9">
         <v>-4.4623714561606054</v>
       </c>
-      <c r="AA30" s="13">
-        <v>418</v>
+      <c r="AA30">
+        <v>442</v>
       </c>
       <c r="AB30" s="9">
         <v>2.9821240395715352</v>
@@ -3293,26 +3416,31 @@
       <c r="F31" s="9">
         <v>0.127</v>
       </c>
-      <c r="G31" s="5">
-        <v>0</v>
-      </c>
-      <c r="H31" s="5">
-        <v>1</v>
-      </c>
-      <c r="I31" s="5">
-        <v>0</v>
-      </c>
-      <c r="J31" s="5">
-        <v>0</v>
-      </c>
-      <c r="K31" s="5">
+      <c r="G31" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="14">
+        <f t="shared" si="3"/>
+        <v>1.8513782324524011E-2</v>
+      </c>
+      <c r="I31" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L31" s="5">
         <v>0</v>
       </c>
       <c r="M31" s="5">
-        <v>0.1</v>
+        <v>9.8039215686274508E-2</v>
       </c>
       <c r="N31" s="5">
         <v>0</v>
@@ -3333,23 +3461,23 @@
         <v>86.333333333333329</v>
       </c>
       <c r="T31" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U31" s="5">
-        <f t="shared" ref="U31:X31" si="28">SUM(H29:H31)</f>
-        <v>2</v>
+        <f t="shared" ref="U31:X31" si="32">SUM(H29:H31)</f>
+        <v>2.2136970730321111E-2</v>
       </c>
       <c r="V31" s="5">
-        <f t="shared" si="28"/>
-        <v>1</v>
+        <f t="shared" si="32"/>
+        <v>0</v>
       </c>
       <c r="W31" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="X31" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Y31" s="9">
@@ -3358,8 +3486,8 @@
       <c r="Z31" s="9">
         <v>1.8229087636707599</v>
       </c>
-      <c r="AA31" s="13">
-        <v>492</v>
+      <c r="AA31">
+        <v>502</v>
       </c>
       <c r="AB31" s="9">
         <v>0.97883518386852897</v>
@@ -3384,19 +3512,24 @@
       <c r="F32" s="9">
         <v>0.72799999999999998</v>
       </c>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32" s="5">
-        <v>0</v>
-      </c>
-      <c r="I32" s="5">
-        <v>0</v>
-      </c>
-      <c r="J32" s="5">
-        <v>0</v>
-      </c>
-      <c r="K32" s="5">
+      <c r="G32" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="14">
+        <f t="shared" si="3"/>
+        <v>1.1253196930946292E-2</v>
+      </c>
+      <c r="I32" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L32" s="5">
@@ -3424,23 +3557,23 @@
         <v>104.66666666666667</v>
       </c>
       <c r="T32" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U32" s="5">
-        <f t="shared" ref="U32:X32" si="29">SUM(H30:H32)</f>
-        <v>2</v>
+        <f t="shared" ref="U32:X32" si="33">SUM(H30:H32)</f>
+        <v>3.33901676612674E-2</v>
       </c>
       <c r="V32" s="5">
-        <f t="shared" si="29"/>
-        <v>1</v>
+        <f t="shared" si="33"/>
+        <v>0</v>
       </c>
       <c r="W32" s="5">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="X32" s="5">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="Y32" s="9">
@@ -3449,8 +3582,8 @@
       <c r="Z32" s="9">
         <v>0.314466430287693</v>
       </c>
-      <c r="AA32" s="13">
-        <v>608</v>
+      <c r="AA32">
+        <v>611</v>
       </c>
       <c r="AB32" s="9">
         <v>0.70593726610420804</v>
@@ -3475,26 +3608,31 @@
       <c r="F33" s="9">
         <v>-0.308</v>
       </c>
-      <c r="G33" s="5">
-        <v>0</v>
-      </c>
-      <c r="H33" s="5">
-        <v>1</v>
-      </c>
-      <c r="I33" s="5">
-        <v>0</v>
-      </c>
-      <c r="J33" s="5">
-        <v>0</v>
-      </c>
-      <c r="K33" s="5">
+      <c r="G33" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="14">
+        <f t="shared" si="3"/>
+        <v>1.1586452762923352E-2</v>
+      </c>
+      <c r="I33" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L33" s="5">
         <v>0</v>
       </c>
       <c r="M33" s="5">
-        <v>0.03</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="N33" s="5">
         <v>0</v>
@@ -3515,23 +3653,23 @@
         <v>54</v>
       </c>
       <c r="T33" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U33" s="5">
-        <f t="shared" ref="U33:X33" si="30">SUM(H31:H33)</f>
-        <v>2</v>
+        <f t="shared" ref="U33:X33" si="34">SUM(H31:H33)</f>
+        <v>4.1353432018393657E-2</v>
       </c>
       <c r="V33" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W33" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X33" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="Y33" s="9">
@@ -3540,8 +3678,8 @@
       <c r="Z33" s="9">
         <v>4.5971793245503498</v>
       </c>
-      <c r="AA33" s="13">
-        <v>674</v>
+      <c r="AA33">
+        <v>677</v>
       </c>
       <c r="AB33" s="9">
         <v>-0.90814805445389657</v>
@@ -3566,26 +3704,31 @@
       <c r="F34" s="9">
         <v>-0.749</v>
       </c>
-      <c r="G34" s="5">
-        <v>1</v>
-      </c>
-      <c r="H34" s="5">
-        <v>1</v>
-      </c>
-      <c r="I34" s="5">
-        <v>0</v>
-      </c>
-      <c r="J34" s="5">
-        <v>0</v>
-      </c>
-      <c r="K34" s="5">
+      <c r="G34" s="14">
+        <f t="shared" si="2"/>
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="H34" s="14">
+        <f t="shared" si="3"/>
+        <v>8.5858585858585856E-3</v>
+      </c>
+      <c r="I34" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L34" s="5">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M34" s="5">
-        <v>0.03</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="N34" s="5">
         <v>0</v>
@@ -3606,23 +3749,23 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T34" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="U34" s="5">
-        <f t="shared" ref="U34:X34" si="31">SUM(H32:H34)</f>
-        <v>2</v>
+        <f t="shared" ref="U34:X34" si="35">SUM(H32:H34)</f>
+        <v>3.1425508279728231E-2</v>
       </c>
       <c r="V34" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="W34" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="X34" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y34" s="9">
@@ -3631,7 +3774,7 @@
       <c r="Z34" s="9">
         <v>4.9054919553647247</v>
       </c>
-      <c r="AA34" s="13">
+      <c r="AA34">
         <v>831</v>
       </c>
       <c r="AB34" s="9">
@@ -3657,19 +3800,24 @@
       <c r="F35" s="9">
         <v>-1.125</v>
       </c>
-      <c r="G35" s="5">
-        <v>0</v>
-      </c>
-      <c r="H35" s="5">
-        <v>0</v>
-      </c>
-      <c r="I35" s="5">
-        <v>0</v>
-      </c>
-      <c r="J35" s="5">
-        <v>0</v>
-      </c>
-      <c r="K35" s="5">
+      <c r="G35" s="14">
+        <f t="shared" si="2"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H35" s="14">
+        <f t="shared" si="3"/>
+        <v>5.3535353535353533E-3</v>
+      </c>
+      <c r="I35" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L35" s="5">
@@ -3697,23 +3845,23 @@
         <v>165.66666666666666</v>
       </c>
       <c r="T35" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>6.6666666666666662E-3</v>
       </c>
       <c r="U35" s="5">
-        <f t="shared" ref="U35:X35" si="32">SUM(H33:H35)</f>
-        <v>2</v>
+        <f t="shared" ref="U35:X35" si="36">SUM(H33:H35)</f>
+        <v>2.5525846702317292E-2</v>
       </c>
       <c r="V35" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W35" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="X35" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Y35" s="9">
@@ -3722,8 +3870,8 @@
       <c r="Z35" s="9">
         <v>-4.3319024391373304</v>
       </c>
-      <c r="AA35" s="13">
-        <v>516</v>
+      <c r="AA35">
+        <v>519</v>
       </c>
       <c r="AB35" s="9">
         <v>-5.3832213694813404</v>
@@ -3748,26 +3896,31 @@
       <c r="F36" s="9">
         <v>-1.8620000000000001</v>
       </c>
-      <c r="G36" s="5">
-        <v>0</v>
-      </c>
-      <c r="H36" s="5">
-        <v>1</v>
-      </c>
-      <c r="I36" s="5">
-        <v>0</v>
-      </c>
-      <c r="J36" s="5">
-        <v>0</v>
-      </c>
-      <c r="K36" s="5">
+      <c r="G36" s="14">
+        <f t="shared" si="2"/>
+        <v>1.666666666666667E-3</v>
+      </c>
+      <c r="H36" s="14">
+        <f t="shared" si="3"/>
+        <v>6.2872628726287271E-3</v>
+      </c>
+      <c r="I36" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L36" s="5">
         <v>0</v>
       </c>
       <c r="M36" s="5">
-        <v>0.02</v>
+        <v>2.4390243902439025E-2</v>
       </c>
       <c r="N36" s="5">
         <v>0</v>
@@ -3788,23 +3941,23 @@
         <v>171.33333333333334</v>
       </c>
       <c r="T36" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="U36" s="5">
-        <f t="shared" ref="U36:X36" si="33">SUM(H34:H36)</f>
-        <v>2</v>
+        <f t="shared" ref="U36:X36" si="37">SUM(H34:H36)</f>
+        <v>2.0226656812022667E-2</v>
       </c>
       <c r="V36" s="5">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="W36" s="5">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="X36" s="5">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="Y36" s="9">
@@ -3813,7 +3966,7 @@
       <c r="Z36" s="9">
         <v>-6.6667644212892396</v>
       </c>
-      <c r="AA36" s="13">
+      <c r="AA36">
         <v>653</v>
       </c>
       <c r="AB36" s="9">
@@ -3839,19 +3992,24 @@
       <c r="F37" s="9">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="G37" s="5">
-        <v>0</v>
-      </c>
-      <c r="H37" s="5">
-        <v>0</v>
-      </c>
-      <c r="I37" s="5">
-        <v>0</v>
-      </c>
-      <c r="J37" s="5">
-        <v>0</v>
-      </c>
-      <c r="K37" s="5">
+      <c r="G37" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="14">
+        <f t="shared" si="3"/>
+        <v>2.4390243902439024E-3</v>
+      </c>
+      <c r="I37" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L37" s="5">
@@ -3879,23 +4037,23 @@
         <v>133.33333333333334</v>
       </c>
       <c r="T37" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>4.1666666666666675E-3</v>
       </c>
       <c r="U37" s="5">
-        <f t="shared" ref="U37:X37" si="34">SUM(H35:H37)</f>
-        <v>1</v>
+        <f t="shared" ref="U37:X37" si="38">SUM(H35:H37)</f>
+        <v>1.4079822616407984E-2</v>
       </c>
       <c r="V37" s="5">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="W37" s="5">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X37" s="5">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Y37" s="9">
@@ -3904,8 +4062,8 @@
       <c r="Z37" s="9">
         <v>-0.75959971101834345</v>
       </c>
-      <c r="AA37" s="13">
-        <v>433</v>
+      <c r="AA37">
+        <v>455</v>
       </c>
       <c r="AB37" s="9">
         <v>-3.9593844720987009E-2</v>
@@ -3930,26 +4088,31 @@
       <c r="F38" s="9">
         <v>-1.0740000000000001</v>
       </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-      <c r="H38" s="5">
-        <v>1</v>
-      </c>
-      <c r="I38" s="5">
-        <v>0</v>
-      </c>
-      <c r="J38" s="5">
-        <v>0</v>
-      </c>
-      <c r="K38" s="5">
+      <c r="G38" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14">
+        <f t="shared" si="3"/>
+        <v>5.7926829268292691E-3</v>
+      </c>
+      <c r="I38" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L38" s="5">
         <v>0</v>
       </c>
       <c r="M38" s="5">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="N38" s="5">
         <v>0</v>
@@ -3970,23 +4133,23 @@
         <v>70</v>
       </c>
       <c r="T38" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1.666666666666667E-3</v>
       </c>
       <c r="U38" s="5">
-        <f t="shared" ref="U38:X38" si="35">SUM(H36:H38)</f>
-        <v>2</v>
+        <f t="shared" ref="U38:X38" si="39">SUM(H36:H38)</f>
+        <v>1.4518970189701899E-2</v>
       </c>
       <c r="V38" s="5">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="W38" s="5">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X38" s="5">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y38" s="9">
@@ -3995,7 +4158,7 @@
       <c r="Z38" s="9">
         <v>-1.5664581156725255</v>
       </c>
-      <c r="AA38" s="13">
+      <c r="AA38">
         <v>719</v>
       </c>
       <c r="AB38" s="9">
@@ -4021,26 +4184,31 @@
       <c r="F39" s="9">
         <v>-1.4319999999999999</v>
       </c>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-      <c r="H39" s="5">
-        <v>1</v>
-      </c>
-      <c r="I39" s="5">
-        <v>0</v>
-      </c>
-      <c r="J39" s="5">
-        <v>0</v>
-      </c>
-      <c r="K39" s="5">
+      <c r="G39" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="14">
+        <f>AVERAGE(0.2*M37,0.3*M38,0.5*M39)</f>
+        <v>7.5505050505050506E-3</v>
+      </c>
+      <c r="I39" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L39" s="5">
         <v>0</v>
       </c>
       <c r="M39" s="5">
-        <v>0.03</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="N39" s="5">
         <v>0</v>
@@ -4061,23 +4229,23 @@
         <v>58.333333333333336</v>
       </c>
       <c r="T39" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U39" s="5">
-        <f t="shared" ref="U39:X39" si="36">SUM(H37:H39)</f>
-        <v>2</v>
+        <f t="shared" ref="U39:X39" si="40">SUM(H37:H39)</f>
+        <v>1.5782212367578222E-2</v>
       </c>
       <c r="V39" s="5">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W39" s="5">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="X39" s="5">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Y39" s="9">
@@ -4086,8 +4254,8 @@
       <c r="Z39" s="9">
         <v>-1.8991672842734699</v>
       </c>
-      <c r="AA39" s="13">
-        <v>753</v>
+      <c r="AA39">
+        <v>758</v>
       </c>
       <c r="AB39" s="9">
         <v>-3.94158080668281</v>
@@ -4112,19 +4280,24 @@
       <c r="F40" s="9">
         <v>-1.115</v>
       </c>
-      <c r="G40" s="5">
-        <v>0</v>
-      </c>
-      <c r="H40" s="5">
-        <v>0</v>
-      </c>
-      <c r="I40" s="5">
-        <v>0</v>
-      </c>
-      <c r="J40" s="5">
-        <v>0</v>
-      </c>
-      <c r="K40" s="5">
+      <c r="G40" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="14">
+        <f t="shared" si="3"/>
+        <v>4.6969696969696969E-3</v>
+      </c>
+      <c r="I40" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L40" s="5">
@@ -4152,23 +4325,23 @@
         <v>103.33333333333333</v>
       </c>
       <c r="T40" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U40" s="5">
-        <f t="shared" ref="U40:X40" si="37">SUM(H38:H40)</f>
-        <v>2</v>
+        <f t="shared" ref="U40:X40" si="41">SUM(H38:H40)</f>
+        <v>1.8040157674304017E-2</v>
       </c>
       <c r="V40" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W40" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="X40" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Y40" s="9">
@@ -4177,8 +4350,8 @@
       <c r="Z40" s="9">
         <v>-2.448511848603375</v>
       </c>
-      <c r="AA40" s="13">
-        <v>826</v>
+      <c r="AA40">
+        <v>830</v>
       </c>
       <c r="AB40" s="9">
         <v>2.6823130452793751</v>
@@ -4203,19 +4376,24 @@
       <c r="F41" s="9">
         <v>0.42599999999999999</v>
       </c>
-      <c r="G41" s="5">
-        <v>0</v>
-      </c>
-      <c r="H41" s="5">
-        <v>0</v>
-      </c>
-      <c r="I41" s="5">
-        <v>0</v>
-      </c>
-      <c r="J41" s="5">
-        <v>0</v>
-      </c>
-      <c r="K41" s="5">
+      <c r="G41" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="14">
+        <f t="shared" si="3"/>
+        <v>2.0202020202020206E-3</v>
+      </c>
+      <c r="I41" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="14">
+        <f>AVERAGE(0.2*P39,0.3*P40,0.5*P41)</f>
         <v>0</v>
       </c>
       <c r="L41" s="5">
@@ -4243,23 +4421,23 @@
         <v>158</v>
       </c>
       <c r="T41" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U41" s="5">
-        <f t="shared" ref="U41:X41" si="38">SUM(H39:H41)</f>
-        <v>1</v>
+        <f t="shared" ref="U41:X41" si="42">SUM(H39:H41)</f>
+        <v>1.4267676767676768E-2</v>
       </c>
       <c r="V41" s="5">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="W41" s="5">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="X41" s="5">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="Y41" s="9">
@@ -4268,8 +4446,8 @@
       <c r="Z41" s="9">
         <v>-2.8938079755209851</v>
       </c>
-      <c r="AA41" s="13">
-        <v>880</v>
+      <c r="AA41">
+        <v>883</v>
       </c>
       <c r="AB41" s="9">
         <v>-4.9758346309216446</v>
@@ -4294,26 +4472,31 @@
       <c r="F42" s="9">
         <v>1.3260000000000001</v>
       </c>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
-      <c r="H42" s="5">
-        <v>1</v>
-      </c>
-      <c r="I42" s="5">
-        <v>0</v>
-      </c>
-      <c r="J42" s="5">
-        <v>0</v>
-      </c>
-      <c r="K42" s="5">
+      <c r="G42" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="14">
+        <f t="shared" si="3"/>
+        <v>4.6296296296296294E-3</v>
+      </c>
+      <c r="I42" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L42" s="5">
         <v>0</v>
       </c>
       <c r="M42" s="5">
-        <v>0.03</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="N42" s="5">
         <v>0</v>
@@ -4334,23 +4517,23 @@
         <v>108</v>
       </c>
       <c r="T42" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U42" s="5">
-        <f t="shared" ref="U42:X42" si="39">SUM(H40:H42)</f>
-        <v>1</v>
+        <f t="shared" ref="U42:X42" si="43">SUM(H40:H42)</f>
+        <v>1.1346801346801346E-2</v>
       </c>
       <c r="V42" s="5">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="W42" s="5">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="X42" s="5">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Y42" s="9">
@@ -4359,8 +4542,8 @@
       <c r="Z42" s="9">
         <v>1.40123084918149</v>
       </c>
-      <c r="AA42" s="13">
-        <v>777</v>
+      <c r="AA42">
+        <v>781</v>
       </c>
       <c r="AB42" s="9">
         <v>8.728865487872115</v>
@@ -4385,26 +4568,31 @@
       <c r="F43" s="9">
         <v>1.571</v>
       </c>
-      <c r="G43" s="5">
-        <v>1</v>
-      </c>
-      <c r="H43" s="5">
-        <v>1</v>
-      </c>
-      <c r="I43" s="5">
-        <v>1</v>
-      </c>
-      <c r="J43" s="5">
-        <v>0</v>
-      </c>
-      <c r="K43" s="5">
+      <c r="G43" s="14">
+        <f t="shared" si="2"/>
+        <v>4.2735042735042731E-3</v>
+      </c>
+      <c r="H43" s="14">
+        <f t="shared" si="3"/>
+        <v>1.5123456790123455E-2</v>
+      </c>
+      <c r="I43" s="14">
+        <f>AVERAGE(0.2*N41,0.3*N42,0.5*N43)</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="J43" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L43" s="5">
-        <v>0.03</v>
+        <v>2.564102564102564E-2</v>
       </c>
       <c r="M43" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>7.407407407407407E-2</v>
       </c>
       <c r="N43" s="5">
         <v>0.1</v>
@@ -4425,23 +4613,23 @@
         <v>157.33333333333334</v>
       </c>
       <c r="T43" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>4.2735042735042731E-3</v>
       </c>
       <c r="U43" s="5">
-        <f t="shared" ref="U43:X43" si="40">SUM(H41:H43)</f>
-        <v>2</v>
+        <f t="shared" ref="U43:X43" si="44">SUM(H41:H43)</f>
+        <v>2.1773288439955105E-2</v>
       </c>
       <c r="V43" s="5">
-        <f t="shared" si="40"/>
-        <v>1</v>
+        <f t="shared" si="44"/>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="W43" s="5">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="X43" s="5">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Y43" s="9">
@@ -4450,8 +4638,8 @@
       <c r="Z43" s="9">
         <v>3.9882261960460097</v>
       </c>
-      <c r="AA43" s="13">
-        <v>825</v>
+      <c r="AA43">
+        <v>826</v>
       </c>
       <c r="AB43" s="9">
         <v>4.6032079036796496</v>
@@ -4476,26 +4664,31 @@
       <c r="F44" s="9">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G44" s="5">
-        <v>0</v>
-      </c>
-      <c r="H44" s="5">
-        <v>1</v>
-      </c>
-      <c r="I44" s="5">
-        <v>1</v>
-      </c>
-      <c r="J44" s="5">
-        <v>0</v>
-      </c>
-      <c r="K44" s="5">
+      <c r="G44" s="14">
+        <f t="shared" si="2"/>
+        <v>2.5641025641025641E-3</v>
+      </c>
+      <c r="H44" s="14">
+        <f t="shared" si="3"/>
+        <v>2.3544973544973546E-2</v>
+      </c>
+      <c r="I44" s="14">
+        <f t="shared" si="4"/>
+        <v>5.1666666666666666E-2</v>
+      </c>
+      <c r="J44" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L44" s="5">
         <v>0</v>
       </c>
       <c r="M44" s="5">
-        <v>0.09</v>
+        <v>8.5714285714285715E-2</v>
       </c>
       <c r="N44" s="5">
         <v>0.25</v>
@@ -4516,23 +4709,23 @@
         <v>108.33333333333333</v>
       </c>
       <c r="T44" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>6.8376068376068376E-3</v>
       </c>
       <c r="U44" s="5">
-        <f t="shared" ref="U44:X44" si="41">SUM(H42:H44)</f>
-        <v>3</v>
+        <f t="shared" ref="U44:X44" si="45">SUM(H42:H44)</f>
+        <v>4.3298059964726632E-2</v>
       </c>
       <c r="V44" s="5">
         <f>SUM(I42:I44)</f>
-        <v>2</v>
+        <v>6.8333333333333329E-2</v>
       </c>
       <c r="W44" s="5">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="X44" s="5">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y44" s="9">
@@ -4541,8 +4734,8 @@
       <c r="Z44" s="9">
         <v>3.7462448286140551</v>
       </c>
-      <c r="AA44" s="13">
-        <v>703</v>
+      <c r="AA44">
+        <v>719</v>
       </c>
       <c r="AB44" s="9">
         <v>2.6078631351677197</v>
@@ -4567,26 +4760,31 @@
       <c r="F45" s="9">
         <v>-0.77800000000000002</v>
       </c>
-      <c r="G45" s="5">
-        <v>0</v>
-      </c>
-      <c r="H45" s="5">
-        <v>1</v>
-      </c>
-      <c r="I45" s="5">
-        <v>0</v>
-      </c>
-      <c r="J45" s="5">
-        <v>0</v>
-      </c>
-      <c r="K45" s="5">
+      <c r="G45" s="14">
+        <f t="shared" si="2"/>
+        <v>1.7094017094017094E-3</v>
+      </c>
+      <c r="H45" s="14">
+        <f t="shared" si="3"/>
+        <v>1.7783204449871113E-2</v>
+      </c>
+      <c r="I45" s="14">
+        <f t="shared" si="4"/>
+        <v>3.1666666666666669E-2</v>
+      </c>
+      <c r="J45" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L45" s="5">
         <v>0</v>
       </c>
       <c r="M45" s="5">
-        <v>0.03</v>
+        <v>2.564102564102564E-2</v>
       </c>
       <c r="N45" s="5">
         <v>0</v>
@@ -4607,23 +4805,23 @@
         <v>111.66666666666667</v>
       </c>
       <c r="T45" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>8.5470085470085479E-3</v>
       </c>
       <c r="U45" s="5">
-        <f t="shared" ref="U45:X45" si="42">SUM(H43:H45)</f>
-        <v>3</v>
+        <f t="shared" ref="U45:X45" si="46">SUM(H43:H45)</f>
+        <v>5.6451634784968119E-2</v>
       </c>
       <c r="V45" s="5">
-        <f t="shared" si="42"/>
-        <v>2</v>
+        <f t="shared" si="46"/>
+        <v>0.1</v>
       </c>
       <c r="W45" s="5">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X45" s="5">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Y45" s="9">
@@ -4632,8 +4830,8 @@
       <c r="Z45" s="9">
         <v>2.4873387255813197</v>
       </c>
-      <c r="AA45" s="13">
-        <v>1092</v>
+      <c r="AA45">
+        <v>1103</v>
       </c>
       <c r="AB45" s="9">
         <v>-0.32915289173666251</v>
@@ -4658,26 +4856,31 @@
       <c r="F46" s="9">
         <v>-0.313</v>
       </c>
-      <c r="G46" s="5">
-        <v>1</v>
-      </c>
-      <c r="H46" s="5">
-        <v>1</v>
-      </c>
-      <c r="I46" s="5">
-        <v>1</v>
-      </c>
-      <c r="J46" s="5">
-        <v>0</v>
-      </c>
-      <c r="K46" s="5">
+      <c r="G46" s="14">
+        <f t="shared" si="2"/>
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="H46" s="14">
+        <f t="shared" si="3"/>
+        <v>3.0017518713170887E-2</v>
+      </c>
+      <c r="I46" s="14">
+        <f t="shared" si="4"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J46" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K46" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L46" s="5">
-        <v>0.03</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="M46" s="5">
-        <v>0.13</v>
+        <v>0.13043478260869565</v>
       </c>
       <c r="N46" s="5">
         <v>0.4</v>
@@ -4698,23 +4901,23 @@
         <v>96</v>
       </c>
       <c r="T46" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>9.8290598290598288E-3</v>
       </c>
       <c r="U46" s="5">
-        <f t="shared" ref="U46:X46" si="43">SUM(H44:H46)</f>
-        <v>3</v>
+        <f t="shared" ref="U46:X46" si="47">SUM(H44:H46)</f>
+        <v>7.1345696708015549E-2</v>
       </c>
       <c r="V46" s="5">
-        <f t="shared" si="43"/>
-        <v>2</v>
+        <f t="shared" si="47"/>
+        <v>0.16666666666666669</v>
       </c>
       <c r="W46" s="5">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="X46" s="5">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y46" s="9">
@@ -4723,7 +4926,7 @@
       <c r="Z46" s="9">
         <v>0.37488515661695349</v>
       </c>
-      <c r="AA46" s="13">
+      <c r="AA46">
         <v>941</v>
       </c>
       <c r="AB46" s="9">
@@ -4749,19 +4952,24 @@
       <c r="F47" s="9">
         <v>-1.6439999999999999</v>
       </c>
-      <c r="G47" s="5">
-        <v>0</v>
-      </c>
-      <c r="H47" s="5">
-        <v>1</v>
-      </c>
-      <c r="I47" s="5">
-        <v>0</v>
-      </c>
-      <c r="J47" s="5">
-        <v>0</v>
-      </c>
-      <c r="K47" s="5">
+      <c r="G47" s="14">
+        <f t="shared" si="2"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="H47" s="14">
+        <f t="shared" si="3"/>
+        <v>5.6419546636937941E-2</v>
+      </c>
+      <c r="I47" s="14">
+        <f>AVERAGE(0.2*N45,0.3*N46,0.5*N47)</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="J47" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K47" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L47" s="5">
@@ -4771,7 +4979,7 @@
         <v>0.25</v>
       </c>
       <c r="N47" s="5">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="O47" s="5">
         <v>0</v>
@@ -4789,23 +4997,23 @@
         <v>100</v>
       </c>
       <c r="T47" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>1.0598290598290599E-2</v>
       </c>
       <c r="U47" s="5">
-        <f t="shared" ref="U47:X47" si="44">SUM(H45:H47)</f>
-        <v>3</v>
+        <f t="shared" ref="U47:X47" si="48">SUM(H45:H47)</f>
+        <v>0.10422026979997995</v>
       </c>
       <c r="V47" s="5">
-        <f t="shared" si="44"/>
-        <v>1</v>
+        <f t="shared" si="48"/>
+        <v>0.21499999999999997</v>
       </c>
       <c r="W47" s="5">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="X47" s="5">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="Y47" s="9">
@@ -4814,8 +5022,8 @@
       <c r="Z47" s="9">
         <v>5.6784310454138645</v>
       </c>
-      <c r="AA47" s="13">
-        <v>1058</v>
+      <c r="AA47">
+        <v>1059</v>
       </c>
       <c r="AB47" s="9">
         <v>2.0080743350620982</v>
@@ -4840,29 +5048,34 @@
       <c r="F48" s="9">
         <v>-1.601</v>
       </c>
-      <c r="G48" s="5">
-        <v>0</v>
-      </c>
-      <c r="H48" s="5">
-        <v>1</v>
-      </c>
-      <c r="I48" s="5">
-        <v>1</v>
-      </c>
-      <c r="J48" s="5">
-        <v>0</v>
-      </c>
-      <c r="K48" s="5">
+      <c r="G48" s="14">
+        <f t="shared" si="2"/>
+        <v>9.1666666666666667E-3</v>
+      </c>
+      <c r="H48" s="14">
+        <f t="shared" si="3"/>
+        <v>9.7798216276477154E-2</v>
+      </c>
+      <c r="I48" s="14">
+        <f t="shared" si="4"/>
+        <v>0.11822222222222223</v>
+      </c>
+      <c r="J48" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K48" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L48" s="5">
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="M48" s="5">
-        <v>0.38</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="N48" s="5">
-        <v>0.33</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="O48" s="5">
         <v>0</v>
@@ -4880,23 +5093,23 @@
         <v>94.666666666666671</v>
       </c>
       <c r="T48" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>1.8055555555555554E-2</v>
       </c>
       <c r="U48" s="5">
-        <f t="shared" ref="U48:X48" si="45">SUM(H46:H48)</f>
-        <v>3</v>
+        <f t="shared" ref="U48:X48" si="49">SUM(H46:H48)</f>
+        <v>0.18423528162658598</v>
       </c>
       <c r="V48" s="5">
-        <f t="shared" si="45"/>
-        <v>2</v>
+        <f t="shared" si="49"/>
+        <v>0.30155555555555558</v>
       </c>
       <c r="W48" s="5">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="X48" s="5">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Y48" s="9">
@@ -4905,8 +5118,8 @@
       <c r="Z48" s="9">
         <v>3.0639952044373198</v>
       </c>
-      <c r="AA48" s="13">
-        <v>1129</v>
+      <c r="AA48">
+        <v>1131</v>
       </c>
       <c r="AB48" s="9">
         <v>-3.5344920110967797</v>
@@ -4931,29 +5144,34 @@
       <c r="F49" s="9">
         <v>-1.5720000000000001</v>
       </c>
-      <c r="G49" s="5">
-        <v>0</v>
-      </c>
-      <c r="H49" s="5">
-        <v>1</v>
-      </c>
-      <c r="I49" s="5">
-        <v>1</v>
-      </c>
-      <c r="J49" s="5">
-        <v>0</v>
-      </c>
-      <c r="K49" s="5">
+      <c r="G49" s="14">
+        <f t="shared" si="2"/>
+        <v>8.9285714285714281E-3</v>
+      </c>
+      <c r="H49" s="14">
+        <f t="shared" si="3"/>
+        <v>9.0215924426450753E-2</v>
+      </c>
+      <c r="I49" s="14">
+        <f t="shared" si="4"/>
+        <v>9.5794871794871783E-2</v>
+      </c>
+      <c r="J49" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K49" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L49" s="5">
-        <v>0.03</v>
+        <v>2.8571428571428571E-2</v>
       </c>
       <c r="M49" s="5">
-        <v>0.21</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="N49" s="5">
-        <v>0.23</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="O49" s="5">
         <v>0</v>
@@ -4971,23 +5189,23 @@
         <v>225.66666666666666</v>
       </c>
       <c r="T49" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2.1428571428571429E-2</v>
       </c>
       <c r="U49" s="5">
-        <f t="shared" ref="U49:X49" si="46">SUM(H47:H49)</f>
-        <v>3</v>
+        <f t="shared" ref="U49:X49" si="50">SUM(H47:H49)</f>
+        <v>0.24443368733986587</v>
       </c>
       <c r="V49" s="5">
         <f>SUM(I47:I49)</f>
-        <v>2</v>
+        <v>0.31401709401709399</v>
       </c>
       <c r="W49" s="5">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="X49" s="5">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="Y49" s="9">
@@ -4996,7 +5214,7 @@
       <c r="Z49" s="9">
         <v>-2.7682281116995551</v>
       </c>
-      <c r="AA49" s="13">
+      <c r="AA49">
         <v>1256</v>
       </c>
       <c r="AB49" s="9">
@@ -5022,35 +5240,40 @@
       <c r="F50" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="5">
-        <v>1</v>
-      </c>
-      <c r="H50" s="5">
-        <v>1</v>
-      </c>
-      <c r="I50" s="5">
-        <v>1</v>
-      </c>
-      <c r="J50" s="5">
-        <v>0</v>
-      </c>
-      <c r="K50" s="5">
-        <v>0</v>
-      </c>
-      <c r="L50" t="s">
-        <v>6</v>
-      </c>
-      <c r="M50" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="N50" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="O50" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="P50" s="9" t="s">
-        <v>6</v>
+      <c r="G50" s="14">
+        <f>AVERAGE(0.2*L48,0.3*L49,0.5*L50)</f>
+        <v>1.0020885547201335E-2</v>
+      </c>
+      <c r="H50" s="14">
+        <f t="shared" si="3"/>
+        <v>5.3940034031567198E-2</v>
+      </c>
+      <c r="I50" s="14">
+        <f>AVERAGE(0.2*N48,0.3*N49,0.5*N50)</f>
+        <v>5.9188034188034193E-2</v>
+      </c>
+      <c r="J50" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K50" s="14">
+        <f>AVERAGE(0.2*P48,0.3*P49,0.5*P50)</f>
+        <v>0</v>
+      </c>
+      <c r="L50" s="5">
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="M50" s="13">
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="N50" s="13">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="O50" s="9">
+        <v>0</v>
+      </c>
+      <c r="P50" s="9">
+        <v>0</v>
       </c>
       <c r="Q50" s="9" t="s">
         <v>6</v>
@@ -5063,22 +5286,22 @@
       </c>
       <c r="T50" s="5">
         <f>SUM(G48:G50)</f>
-        <v>1</v>
+        <v>2.8116123642439428E-2</v>
       </c>
       <c r="U50" s="5">
-        <f t="shared" ref="U50" si="47">SUM(H48:H50)</f>
-        <v>3</v>
+        <f t="shared" ref="U50" si="51">SUM(H48:H50)</f>
+        <v>0.2419541747344951</v>
       </c>
       <c r="V50" s="5">
         <f>SUM(I48:I50)</f>
-        <v>3</v>
+        <v>0.27320512820512821</v>
       </c>
       <c r="W50" s="5">
-        <f t="shared" ref="W50" si="48">SUM(J48:J50)</f>
+        <f t="shared" ref="W50" si="52">SUM(J48:J50)</f>
         <v>0</v>
       </c>
       <c r="X50" s="5">
-        <f t="shared" ref="X50" si="49">SUM(K48:K50)</f>
+        <f t="shared" ref="X50" si="53">SUM(K48:K50)</f>
         <v>0</v>
       </c>
       <c r="Y50" s="9" t="s">
@@ -5087,8 +5310,8 @@
       <c r="Z50" s="9">
         <v>-4.2022302358251196</v>
       </c>
-      <c r="AA50" s="14">
-        <v>1200</v>
+      <c r="AA50">
+        <v>1046</v>
       </c>
       <c r="AB50" s="9">
         <v>-1.52761457526795</v>

</xml_diff>